<commit_message>
testing with Transformers - GPT2
</commit_message>
<xml_diff>
--- a/Role_Rules.xlsx
+++ b/Role_Rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27221"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unlvnevada-my.sharepoint.com/personal/nguyed21_unlv_nevada_edu/Documents/EMMA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{894640C0-A031-FE44-A8AA-55F5DCFA2BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40B2E812-ACF9-7E46-8752-B439A7418EBA}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{894640C0-A031-FE44-A8AA-55F5DCFA2BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F53162B-6756-47F6-BED0-DE61A6AED104}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24580" xr2:uid="{AD1CB273-59D2-2B46-B1AF-F72CDFA947D0}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24580" firstSheet="1" activeTab="1" xr2:uid="{AD1CB273-59D2-2B46-B1AF-F72CDFA947D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Roles&amp;Rules" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Sub-team</t>
   </si>
@@ -107,6 +107,11 @@
 Maintain team cloud storage</t>
   </si>
   <si>
+    <t>Gantt chart
+Contribution report
+Meeting minutes</t>
+  </si>
+  <si>
     <t>Editor</t>
   </si>
   <si>
@@ -176,22 +181,38 @@
     <t>Requirements</t>
   </si>
   <si>
+    <t>Critical thinking, programming</t>
+  </si>
+  <si>
+    <t>Time management</t>
+  </si>
+  <si>
+    <t>Attention to detail, critical thinking</t>
+  </si>
+  <si>
     <t>Your skills</t>
   </si>
   <si>
+    <t>Programming, attention to detail</t>
+  </si>
+  <si>
     <t>Your experience</t>
   </si>
   <si>
-    <t>Gantt chart
-Contribution report
-Meeting minutes</t>
+    <t>Computer science, machine learning projects, other computer science projects</t>
+  </si>
+  <si>
+    <t>Add/change</t>
+  </si>
+  <si>
+    <t>I think there should be a role dedicated to creating the solution and relying on the tech researcher's research</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,10 +372,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -656,21 +673,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6317CB5F-1611-2843-A8DC-D14C01AEFBA6}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.125" style="1" customWidth="1"/>
     <col min="5" max="6" width="18.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="7" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="17.100000000000001">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -687,7 +704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="51">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -702,7 +719,7 @@
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="64.5">
       <c r="A3" s="13"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -715,7 +732,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="51">
       <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>12</v>
@@ -728,7 +745,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="48.75">
       <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
@@ -739,75 +756,75 @@
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="51">
       <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="17.100000000000001">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
     </row>
-    <row r="11" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A11" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="17.100000000000001">
       <c r="A12" s="16"/>
       <c r="B12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="16"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
@@ -817,115 +834,115 @@
         <v>7024709533</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="17.100000000000001">
       <c r="A14" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="33.950000000000003">
       <c r="A15" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
@@ -945,50 +962,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6AA2C2-EBCD-4946-B11D-18B35FA0B7F5}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="22.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.5">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5">
       <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1004,43 +1053,43 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1056,43 +1105,43 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1108,43 +1157,43 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>